<commit_message>
File Renaming and update to Roster
</commit_message>
<xml_diff>
--- a/Senate Judiciary 114th.xlsx
+++ b/Senate Judiciary 114th.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23265" windowHeight="10506" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23265" windowHeight="10506"/>
   </bookViews>
   <sheets>
-    <sheet name="Senate Judiciary Committee" sheetId="4" r:id="rId1"/>
-    <sheet name="Pyramids 114th Senate Judiciary" sheetId="2" r:id="rId2"/>
+    <sheet name="The Roster" sheetId="4" r:id="rId1"/>
+    <sheet name="Seniority Pyramid" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -464,15 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,6 +499,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,16 +826,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5546875" customWidth="1"/>
     <col min="4" max="4" width="5.44140625" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -850,7 +852,7 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1"/>
@@ -917,7 +919,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1062,7 +1064,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1183,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1204,66 +1206,66 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.2" x14ac:dyDescent="0.5">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="15.65" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15.65" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="28.2" x14ac:dyDescent="0.5">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="45.7" thickBot="1" x14ac:dyDescent="0.35">
@@ -1300,11 +1302,11 @@
       <c r="A9" s="31"/>
       <c r="B9" s="26"/>
       <c r="C9" s="26"/>
-      <c r="D9" s="41"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="27">
         <v>1975</v>
       </c>
-      <c r="F9" s="42"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
       <c r="I9" s="18"/>
@@ -1317,10 +1319,10 @@
       <c r="E10" s="15">
         <v>1977</v>
       </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="45"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
       <c r="L10" s="2"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -1331,9 +1333,9 @@
       <c r="E11" s="12">
         <v>1979</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="47"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
       <c r="I11" s="19"/>
       <c r="L11" s="23"/>
     </row>
@@ -1347,7 +1349,7 @@
       <c r="C12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="49"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="11">
         <v>1981</v>
       </c>
@@ -1412,11 +1414,11 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="42"/>
+      <c r="D17" s="39"/>
       <c r="E17" s="10">
         <v>1991</v>
       </c>
-      <c r="F17" s="42"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
@@ -1425,11 +1427,11 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="49"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="10">
         <v>1993</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="45"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="9"/>
@@ -1468,7 +1470,7 @@
       <c r="E21" s="10">
         <v>1999</v>
       </c>
-      <c r="F21" s="42"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
@@ -1481,7 +1483,7 @@
       <c r="E22" s="10">
         <v>2001</v>
       </c>
-      <c r="F22" s="48"/>
+      <c r="F22" s="45"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
@@ -1503,11 +1505,11 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="42"/>
+      <c r="D24" s="39"/>
       <c r="E24" s="10">
         <v>2005</v>
       </c>
-      <c r="F24" s="42"/>
+      <c r="F24" s="39"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="9"/>
@@ -1516,11 +1518,11 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="50"/>
+      <c r="D25" s="47"/>
       <c r="E25" s="10">
         <v>2007</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="9"/>
@@ -1529,11 +1531,11 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="50"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="10">
         <v>2009</v>
       </c>
-      <c r="F26" s="42"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="9"/>
@@ -1542,11 +1544,11 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="51"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="10">
         <v>2011</v>
       </c>
-      <c r="F27" s="48"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="9"/>
@@ -1559,7 +1561,7 @@
       <c r="E28" s="10">
         <v>2013</v>
       </c>
-      <c r="F28" s="42"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="9"/>
@@ -1572,7 +1574,7 @@
       <c r="E29" s="14">
         <v>2015</v>
       </c>
-      <c r="F29" s="48"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="35"/>
       <c r="H29" s="13"/>
       <c r="I29" s="21"/>

</xml_diff>